<commit_message>
changes in concise marksheet
Corr/total marks
</commit_message>
<xml_diff>
--- a/marksheets/1401CB01.xlsx
+++ b/marksheets/1401CB01.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="quiz" sheetId="1" state="visible" r:id="rId1"/>
@@ -83,67 +83,67 @@
     </border>
   </borders>
   <cellStyleXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="6">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="7">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="rtitleStyle" xfId="1"/>
-    <cellStyle hidden="0" name="ltitleStyle" xfId="2"/>
-    <cellStyle hidden="0" name="mtitleStyle" xfId="3"/>
-    <cellStyle hidden="0" name="absoluteStyle" xfId="4"/>
-    <cellStyle hidden="0" name="correctStyle" xfId="5"/>
-    <cellStyle hidden="0" name="incorrectStyle" xfId="6"/>
-    <cellStyle hidden="0" name="normalStyle" xfId="7"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="rtitleStyle" xfId="1" hidden="0"/>
+    <cellStyle name="ltitleStyle" xfId="2" hidden="0"/>
+    <cellStyle name="mtitleStyle" xfId="3" hidden="0"/>
+    <cellStyle name="absoluteStyle" xfId="4" hidden="0"/>
+    <cellStyle name="correctStyle" xfId="5" hidden="0"/>
+    <cellStyle name="incorrectStyle" xfId="6" hidden="0"/>
+    <cellStyle name="normalStyle" xfId="7" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -227,7 +227,7 @@
     <ext cx="6029325" cy="790575"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -542,11 +542,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="18"/>
-    <col customWidth="1" max="2" min="2" width="18"/>
-    <col customWidth="1" max="3" min="3" width="18"/>
-    <col customWidth="1" max="4" min="4" width="18"/>
-    <col customWidth="1" max="5" min="5" width="18"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="5">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>-1</v>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>-14</v>
@@ -667,7 +667,7 @@
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>28/84</t>
+          <t>70/140</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
   <mergeCells count="1">
     <mergeCell ref="A5:E5"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Concise.csv Last column fixed
</commit_message>
<xml_diff>
--- a/marksheets/1401CB01.xlsx
+++ b/marksheets/1401CB01.xlsx
@@ -645,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>-14</v>
+        <v>-28</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">

</xml_diff>

<commit_message>
Excel file total marks error
</commit_message>
<xml_diff>
--- a/marksheets/1401CB01.xlsx
+++ b/marksheets/1401CB01.xlsx
@@ -642,10 +642,10 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>0</v>
@@ -659,15 +659,15 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>-14</v>
+        <v>-28</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>70 / 140</t>
+          <t>28 / 112</t>
         </is>
       </c>
     </row>

</xml_diff>